<commit_message>
Added More Array & Hashing programs
</commit_message>
<xml_diff>
--- a/LeetCode 75.xlsx
+++ b/LeetCode 75.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12615" windowHeight="3795"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Category</t>
   </si>
@@ -133,13 +133,37 @@
     <t>https://leetcode.com/problems/reverse-words-in-a-string/?envType=study-plan-v2&amp;envId=leetcode-75</t>
   </si>
   <si>
+    <t>Increasing Triplet Subsequence</t>
+  </si>
+  <si>
+    <t>Use left and mid pointer to keep track of left and mid value, and anytime left&lt;mid&lt;nums[i] return true</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/increasing-triplet-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
     <t>Two Pointer</t>
   </si>
   <si>
+    <t>Move Zeros</t>
+  </si>
+  <si>
+    <t>Use two pointers as l,r=0,0 and keep switching right pointer if not 0 and increment</t>
+  </si>
+  <si>
     <t>Reverse Vowels in a String</t>
   </si>
   <si>
     <t>create vowel array, make newS using .split(''), make two pointers left and right, and incre/decree them only when vowel is found, or else seperately, return newS.join('')</t>
+  </si>
+  <si>
+    <t>Is Subsequence</t>
+  </si>
+  <si>
+    <t>Create two pointers, both at 0, then keep scanning all the characters one by one from both the arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75</t>
   </si>
 </sst>
 </file>
@@ -147,10 +171,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -169,6 +193,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -177,22 +222,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,21 +272,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,9 +285,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,75 +332,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,109 +346,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,73 +526,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,6 +537,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -532,16 +571,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -551,21 +590,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,16 +604,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,58 +642,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -678,88 +702,88 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1089,10 +1113,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1301,18 +1325,66 @@
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 more programs in Hashing
</commit_message>
<xml_diff>
--- a/LeetCode 75.xlsx
+++ b/LeetCode 75.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="19890" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Category</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/increasing-triplet-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t>Unique Number of Occurences</t>
+  </si>
+  <si>
+    <t>Store occurences in a hashtable, then add those in a hashset to look for duplicate values</t>
+  </si>
+  <si>
+    <t>Unique Number of Occurrences - LeetCode</t>
   </si>
   <si>
     <t>Two Pointer</t>
@@ -172,9 +181,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -193,6 +202,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -201,22 +218,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,45 +286,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -286,6 +303,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -294,14 +325,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,21 +334,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,19 +355,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,163 +535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,17 +549,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,6 +573,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -585,20 +597,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,6 +629,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -628,170 +646,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,7 +1128,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1157,7 +1169,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1174,7 +1186,7 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1191,7 +1203,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1208,7 +1220,7 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1225,7 +1237,7 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1242,7 +1254,7 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1259,7 +1271,7 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1287,7 +1299,7 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1304,7 +1316,7 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1321,7 +1333,7 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1338,56 +1350,88 @@
       <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E14" r:id="rId1" display="Unique Number of Occurrences - LeetCode" tooltip="https://leetcode.com/problems/unique-number-of-occurrences/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E13" r:id="rId2" display="https://leetcode.com/problems/increasing-triplet-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E12" r:id="rId3" display="https://leetcode.com/problems/reverse-words-in-a-string/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E11" r:id="rId4" display="https://leetcode.com/problems/can-place-flowers/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E10" r:id="rId5" display="https://leetcode.com/problems/kids-with-the-greatest-number-of-candies/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://leetcode.com/problems/merge-strings-alternately/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E7" r:id="rId7" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/09Longest%20Consequtive%20string"/>
+    <hyperlink ref="E6" r:id="rId8" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/06%20Product%20of%20Array%20Except%20Self"/>
+    <hyperlink ref="E5" r:id="rId9" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/05%20Top%20K%20Frequent%20Element"/>
+    <hyperlink ref="E4" r:id="rId10" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/03%20Two%20Sums"/>
+    <hyperlink ref="E3" r:id="rId11" display="https://github.com/kunalpal101/NeetCode-DSA/blob/master/Array%20%26%20Hashing/02%20Valid%20Anagram/script.js"/>
+    <hyperlink ref="E2" r:id="rId12" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/01%20Contains%20Duplicate"/>
+    <hyperlink ref="E18" r:id="rId13" display="https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Addes stack to the doc
</commit_message>
<xml_diff>
--- a/LeetCode 75.xlsx
+++ b/LeetCode 75.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7545"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>Category</t>
   </si>
@@ -173,6 +173,36 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Valid Parenthesis</t>
+  </si>
+  <si>
+    <t>Create a stack, and then push for open and pop for close</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parentheses/</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>Create a seperate stack, and maintain the minimum value in it. Also, initialize using this.stack</t>
+  </si>
+  <si>
+    <t>Min Stack - LeetCode</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>Create a stack, and then push the numbers and when operators come perform the operation and push the result</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
   </si>
 </sst>
 </file>
@@ -180,10 +210,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -210,6 +240,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -225,25 +277,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -263,9 +299,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,45 +338,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,49 +385,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,25 +547,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,103 +565,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,11 +579,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,21 +628,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -612,26 +642,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,7 +681,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -663,136 +696,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,10 +1155,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1414,6 +1444,57 @@
       </c>
       <c r="E18" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1431,6 +1512,9 @@
     <hyperlink ref="E3" r:id="rId11" display="https://github.com/kunalpal101/NeetCode-DSA/blob/master/Array%20%26%20Hashing/02%20Valid%20Anagram/script.js"/>
     <hyperlink ref="E2" r:id="rId12" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/01%20Contains%20Duplicate"/>
     <hyperlink ref="E18" r:id="rId13" display="https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E20" r:id="rId14" display="https://leetcode.com/problems/valid-parentheses/" tooltip="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="E21" r:id="rId15" display="Min Stack - LeetCode" tooltip="https://leetcode.com/problems/min-stack/"/>
+    <hyperlink ref="E22" r:id="rId16" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added 2 hashing programs in in LeetCode 75
</commit_message>
<xml_diff>
--- a/LeetCode 75.xlsx
+++ b/LeetCode 75.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="91">
   <si>
     <t>Category</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Link</t>
   </si>
   <si>
+    <t>Time Complexity</t>
+  </si>
+  <si>
+    <t>Space Complexity</t>
+  </si>
+  <si>
     <t>Array &amp; Hashing</t>
   </si>
   <si>
@@ -151,6 +157,36 @@
     <t>Unique Number of Occurrences - LeetCode</t>
   </si>
   <si>
+    <t>Determine if two strings are close</t>
+  </si>
+  <si>
+    <t>Create two hashmaps for letter count, check if all letters are same, make two arrays to get their counts and sort them and check if all counts matches</t>
+  </si>
+  <si>
+    <t>Determine if Two Strings Are Close - LeetCode</t>
+  </si>
+  <si>
+    <t>O(n+m * log(m+n))</t>
+  </si>
+  <si>
+    <t>O(n+m)</t>
+  </si>
+  <si>
+    <t>Equal row and column pairs</t>
+  </si>
+  <si>
+    <t>Create two hashmaps for rows and columns as strings seperated via commas, for result multiply the hashmap value of row &amp; col and add to result</t>
+  </si>
+  <si>
+    <t>Equal Row and Column Pairs - LeetCode</t>
+  </si>
+  <si>
+    <t>O(n*n)</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
     <t>Two Pointer</t>
   </si>
   <si>
@@ -230,6 +266,27 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Reverse a Linked List</t>
+  </si>
+  <si>
+    <t>Create two pointers, prev &amp; next, and assign them values accordingly</t>
+  </si>
+  <si>
+    <t>Reverse Linked List - LeetCode</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Create a third list, and add as per sorted order</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -237,10 +294,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -267,6 +324,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -274,10 +346,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -289,82 +415,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -373,6 +423,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -388,16 +453,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,12 +469,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -430,25 +517,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,13 +583,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,121 +607,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,15 +660,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -641,6 +689,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -652,15 +718,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,7 +765,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -717,9 +777,6 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -729,131 +786,131 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -861,6 +918,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1182,21 +1242,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="23.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="54.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="56.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="115.857142857143" customWidth="1"/>
+    <col min="6" max="6" width="18.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="16.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,367 +1274,453 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1589,13 +1737,17 @@
     <hyperlink ref="E4" r:id="rId10" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/03%20Two%20Sums"/>
     <hyperlink ref="E3" r:id="rId11" display="https://github.com/kunalpal101/NeetCode-DSA/blob/master/Array%20%26%20Hashing/02%20Valid%20Anagram/script.js"/>
     <hyperlink ref="E2" r:id="rId12" display="https://github.com/kunalpal101/NeetCode-DSA/tree/master/Array%20%26%20Hashing/01%20Contains%20Duplicate"/>
-    <hyperlink ref="E18" r:id="rId13" display="https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75"/>
-    <hyperlink ref="E23" r:id="rId14" display="https://leetcode.com/problems/valid-parentheses/" tooltip="https://leetcode.com/problems/valid-parentheses/"/>
-    <hyperlink ref="E24" r:id="rId15" display="Min Stack - LeetCode" tooltip="https://leetcode.com/problems/min-stack/"/>
-    <hyperlink ref="E25" r:id="rId16" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/"/>
-    <hyperlink ref="E19" r:id="rId17" display="Valid Palindrome - LeetCode" tooltip="https://leetcode.com/problems/valid-palindrome/description/"/>
-    <hyperlink ref="E20" r:id="rId18" display="Two Sum II - Input Array Is Sorted - LeetCode" tooltip="https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/"/>
-    <hyperlink ref="E21" r:id="rId19" display="Container With Most Water - LeetCode" tooltip="https://leetcode.com/problems/container-with-most-water/"/>
+    <hyperlink ref="E21" r:id="rId13" display="https://leetcode.com/problems/is-subsequence/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E26" r:id="rId14" display="https://leetcode.com/problems/valid-parentheses/" tooltip="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="E27" r:id="rId15" display="Min Stack - LeetCode" tooltip="https://leetcode.com/problems/min-stack/"/>
+    <hyperlink ref="E28" r:id="rId16" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/"/>
+    <hyperlink ref="E22" r:id="rId17" display="Valid Palindrome - LeetCode" tooltip="https://leetcode.com/problems/valid-palindrome/description/"/>
+    <hyperlink ref="E23" r:id="rId18" display="Two Sum II - Input Array Is Sorted - LeetCode" tooltip="https://leetcode.com/problems/two-sum-ii-input-array-is-sorted/"/>
+    <hyperlink ref="E24" r:id="rId19" display="Container With Most Water - LeetCode" tooltip="https://leetcode.com/problems/container-with-most-water/"/>
+    <hyperlink ref="E31" r:id="rId20" display="Reverse Linked List - LeetCode" tooltip="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="E32" r:id="rId21" display="Merge Two Sorted Lists - LeetCode" tooltip="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="E15" r:id="rId22" display="Determine if Two Strings Are Close - LeetCode" tooltip="https://leetcode.com/problems/determine-if-two-strings-are-close/description/?envType=study-plan-v2&amp;envId=leetcode-75"/>
+    <hyperlink ref="E16" r:id="rId23" display="Equal Row and Column Pairs - LeetCode" tooltip="https://leetcode.com/problems/equal-row-and-column-pairs/?envType=study-plan-v2&amp;envId=leetcode-75"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>